<commit_message>
updated example output implemented lualatex (optional) included margins in plot functions
</commit_message>
<xml_diff>
--- a/example_output/csv_data/ExtremeValues_T_return_Wind.xlsx
+++ b/example_output/csv_data/ExtremeValues_T_return_Wind.xlsx
@@ -443,7 +443,7 @@
         <v>36.2</v>
       </c>
       <c r="D3">
-        <v>38</v>
+        <v>37.9</v>
       </c>
       <c r="E3">
         <v>34.9</v>
@@ -457,10 +457,10 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>39.9</v>
+        <v>39.8</v>
       </c>
       <c r="D4">
-        <v>42.8</v>
+        <v>42.6</v>
       </c>
       <c r="E4">
         <v>37.8</v>
@@ -521,10 +521,10 @@
         <v>33.7</v>
       </c>
       <c r="D3">
-        <v>35.7</v>
+        <v>35.6</v>
       </c>
       <c r="E3">
-        <v>32.1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -541,7 +541,7 @@
         <v>41.3</v>
       </c>
       <c r="E4">
-        <v>35.6</v>
+        <v>35.5</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +585,7 @@
         <v>33.7</v>
       </c>
       <c r="E2">
-        <v>30.7</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -599,7 +599,7 @@
         <v>34.4</v>
       </c>
       <c r="D3">
-        <v>36.5</v>
+        <v>36.6</v>
       </c>
       <c r="E3">
         <v>32.6</v>
@@ -613,13 +613,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>39.5</v>
+        <v>39.4</v>
       </c>
       <c r="D4">
         <v>42.9</v>
       </c>
       <c r="E4">
-        <v>36.7</v>
+        <v>36.6</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +680,7 @@
         <v>33.7</v>
       </c>
       <c r="E3">
-        <v>30.2</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -691,13 +691,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>35.9</v>
+        <v>36</v>
       </c>
       <c r="D4">
-        <v>39.1</v>
+        <v>38.9</v>
       </c>
       <c r="E4">
-        <v>33.6</v>
+        <v>33.4</v>
       </c>
     </row>
   </sheetData>
@@ -738,10 +738,10 @@
         <v>28.1</v>
       </c>
       <c r="D2">
-        <v>29.3</v>
+        <v>29.2</v>
       </c>
       <c r="E2">
-        <v>27.1</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -755,10 +755,10 @@
         <v>29.6</v>
       </c>
       <c r="D3">
-        <v>31.1</v>
+        <v>31.2</v>
       </c>
       <c r="E3">
-        <v>28.3</v>
+        <v>28.4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -769,10 +769,10 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>32.9</v>
+        <v>32.8</v>
       </c>
       <c r="D4">
-        <v>35.3</v>
+        <v>35.4</v>
       </c>
       <c r="E4">
         <v>30.9</v>
@@ -819,7 +819,7 @@
         <v>24.8</v>
       </c>
       <c r="E2">
-        <v>23.2</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -836,7 +836,7 @@
         <v>26.4</v>
       </c>
       <c r="E3">
-        <v>24.2</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -853,7 +853,7 @@
         <v>30</v>
       </c>
       <c r="E4">
-        <v>26.4</v>
+        <v>26.2</v>
       </c>
     </row>
   </sheetData>
@@ -897,7 +897,7 @@
         <v>23.4</v>
       </c>
       <c r="E2">
-        <v>21.2</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -911,7 +911,7 @@
         <v>23.7</v>
       </c>
       <c r="D3">
-        <v>25.4</v>
+        <v>25.3</v>
       </c>
       <c r="E3">
         <v>22.5</v>
@@ -928,7 +928,7 @@
         <v>27.1</v>
       </c>
       <c r="D4">
-        <v>29.8</v>
+        <v>29.6</v>
       </c>
       <c r="E4">
         <v>25.2</v>
@@ -972,10 +972,10 @@
         <v>22.6</v>
       </c>
       <c r="D2">
-        <v>23.7</v>
+        <v>23.8</v>
       </c>
       <c r="E2">
-        <v>21.7</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -986,13 +986,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>24.2</v>
+        <v>24.1</v>
       </c>
       <c r="D3">
-        <v>25.6</v>
+        <v>25.7</v>
       </c>
       <c r="E3">
-        <v>23</v>
+        <v>22.9</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1006,10 +1006,10 @@
         <v>27.5</v>
       </c>
       <c r="D4">
-        <v>29.8</v>
+        <v>29.9</v>
       </c>
       <c r="E4">
-        <v>25.7</v>
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>
@@ -1047,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>23.1</v>
+        <v>23.2</v>
       </c>
       <c r="D2">
         <v>24.2</v>
@@ -1064,10 +1064,10 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>24.6</v>
+        <v>24.7</v>
       </c>
       <c r="D3">
-        <v>26.1</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>23.4</v>
@@ -1084,7 +1084,7 @@
         <v>27.9</v>
       </c>
       <c r="D4">
-        <v>30.3</v>
+        <v>30.1</v>
       </c>
       <c r="E4">
         <v>26.1</v>
@@ -1128,7 +1128,7 @@
         <v>23.5</v>
       </c>
       <c r="D2">
-        <v>24.4</v>
+        <v>24.6</v>
       </c>
       <c r="E2">
         <v>22.7</v>
@@ -1142,10 +1142,10 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>24.8</v>
+        <v>24.9</v>
       </c>
       <c r="D3">
-        <v>26.1</v>
+        <v>26.3</v>
       </c>
       <c r="E3">
         <v>23.8</v>
@@ -1159,13 +1159,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>27.8</v>
+        <v>28</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>30.1</v>
       </c>
       <c r="E4">
-        <v>26.1</v>
+        <v>26.3</v>
       </c>
     </row>
   </sheetData>
@@ -1206,10 +1206,10 @@
         <v>24.5</v>
       </c>
       <c r="D2">
-        <v>25.7</v>
+        <v>25.5</v>
       </c>
       <c r="E2">
-        <v>23.6</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1223,10 +1223,10 @@
         <v>26</v>
       </c>
       <c r="D3">
-        <v>27.6</v>
+        <v>27.4</v>
       </c>
       <c r="E3">
-        <v>24.9</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1237,13 +1237,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>29.4</v>
+        <v>29.3</v>
       </c>
       <c r="D4">
-        <v>31.9</v>
+        <v>31.5</v>
       </c>
       <c r="E4">
-        <v>27.5</v>
+        <v>27.3</v>
       </c>
     </row>
   </sheetData>
@@ -1284,10 +1284,10 @@
         <v>29.2</v>
       </c>
       <c r="D2">
-        <v>30.9</v>
+        <v>30.8</v>
       </c>
       <c r="E2">
-        <v>28</v>
+        <v>27.9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1301,10 +1301,10 @@
         <v>31.3</v>
       </c>
       <c r="D3">
-        <v>33.6</v>
+        <v>33.5</v>
       </c>
       <c r="E3">
-        <v>29.7</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1318,10 +1318,10 @@
         <v>35.9</v>
       </c>
       <c r="D4">
-        <v>39.7</v>
+        <v>39.4</v>
       </c>
       <c r="E4">
-        <v>33.4</v>
+        <v>33.1</v>
       </c>
     </row>
   </sheetData>
@@ -1359,13 +1359,13 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>30.8</v>
+        <v>30.6</v>
       </c>
       <c r="D2">
-        <v>32.1</v>
+        <v>32</v>
       </c>
       <c r="E2">
-        <v>29.6</v>
+        <v>29.5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1376,13 +1376,13 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>32.7</v>
+        <v>32.6</v>
       </c>
       <c r="D3">
-        <v>34.6</v>
+        <v>34.4</v>
       </c>
       <c r="E3">
-        <v>31.2</v>
+        <v>31.1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1393,13 +1393,13 @@
         <v>50</v>
       </c>
       <c r="C4">
-        <v>37</v>
+        <v>36.8</v>
       </c>
       <c r="D4">
-        <v>40</v>
+        <v>39.7</v>
       </c>
       <c r="E4">
-        <v>34.6</v>
+        <v>34.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>